<commit_message>
rename file + fix the bug with forex4you paginator
</commit_message>
<xml_diff>
--- a/resources/БАЗА ДАННЫХ/litefinance/excel/ExtremeGold.xlsx
+++ b/resources/БАЗА ДАННЫХ/litefinance/excel/ExtremeGold.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,39 +498,39 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023.11.29 16:18</t>
+          <t>2023.11.30 11:25</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2043.16</t>
+          <t>2038.04</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023.11.29 16:21</t>
+          <t>2023.11.30 11:37</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2041.43</t>
+          <t>2039.39</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>6,92 USD</t>
+          <t>5,40 USD</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -545,34 +545,34 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023.11.29 09:34</t>
+          <t>2023.11.29 16:49</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2042.5</t>
+          <t>2042.1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023.11.29 16:19</t>
+          <t>2023.11.30 11:21</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2042.04</t>
+          <t>2037.32</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2,76 USD</t>
+          <t>19,12 USD</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -582,39 +582,39 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2023.11.29 15:43</t>
+          <t>2023.11.29 14:52</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2043.16</t>
+          <t>2040.72</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023.11.29 15:54</t>
+          <t>2023.11.30 10:51</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2044.2</t>
+          <t>2039.53</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>4,16 USD</t>
+          <t>7,14 USD</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -624,32 +624,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023.11.29 15:37</t>
+          <t>2023.11.29 16:18</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2044.01</t>
+          <t>2043.16</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023.11.29 15:54</t>
+          <t>2023.11.29 16:21</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2044.3</t>
+          <t>2041.43</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1,74 USD</t>
+          <t>6,92 USD</t>
         </is>
       </c>
     </row>
@@ -666,32 +666,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023.11.29 15:37</t>
+          <t>2023.11.29 09:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2044.02</t>
+          <t>2042.5</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023.11.29 15:54</t>
+          <t>2023.11.29 16:19</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2044.53</t>
+          <t>2042.04</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>3,06 USD</t>
+          <t>2,76 USD</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2043.8</t>
+          <t>2043.16</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -728,19 +728,19 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2044.56</t>
+          <t>2044.2</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>3,04 USD</t>
+          <t>4,16 USD</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -755,12 +755,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023.11.29 15:41</t>
+          <t>2023.11.29 15:37</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2044.17</t>
+          <t>2044.01</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -770,19 +770,19 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2044.68</t>
+          <t>2044.3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2,04 USD</t>
+          <t>1,74 USD</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -797,12 +797,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2023.11.29 15:41</t>
+          <t>2023.11.29 15:37</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2044.2</t>
+          <t>2044.02</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -812,19 +812,19 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2044.59</t>
+          <t>2044.53</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1,56 USD</t>
+          <t>3,06 USD</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -839,12 +839,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023.11.29 15:37</t>
+          <t>2023.11.29 15:43</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2044.03</t>
+          <t>2043.8</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -854,19 +854,19 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2044.51</t>
+          <t>2044.56</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2,88 USD</t>
+          <t>3,04 USD</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -881,12 +881,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2023.11.29 15:37</t>
+          <t>2023.11.29 15:41</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2044</t>
+          <t>2044.17</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -896,12 +896,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2044.67</t>
+          <t>2044.68</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>4,02 USD</t>
+          <t>2,04 USD</t>
         </is>
       </c>
     </row>
@@ -928,29 +928,29 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2044.25</t>
+          <t>2044.2</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2023.11.29 15:41</t>
+          <t>2023.11.29 15:54</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2044.94</t>
+          <t>2044.59</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2,76 USD</t>
+          <t>1,56 USD</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -960,39 +960,39 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2023.11.29 13:19</t>
+          <t>2023.11.29 15:37</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2040.87</t>
+          <t>2044.03</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2023.11.29 14:39</t>
+          <t>2023.11.29 15:54</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2038.11</t>
+          <t>2044.51</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>13,80 USD</t>
+          <t>2,88 USD</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1002,32 +1002,32 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023.11.28 03:34</t>
+          <t>2023.11.29 15:37</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2017.19</t>
+          <t>2044</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2023.11.28 08:50</t>
+          <t>2023.11.29 15:54</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2012.56</t>
+          <t>2044.67</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>23,15 USD</t>
+          <t>4,02 USD</t>
         </is>
       </c>
     </row>
@@ -1044,39 +1044,39 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023.11.28 01:03</t>
+          <t>2023.11.29 15:41</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2017.23</t>
+          <t>2044.25</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2023.11.28 05:04</t>
+          <t>2023.11.29 15:41</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2014.6</t>
+          <t>2044.94</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>10,52 USD</t>
+          <t>2,76 USD</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1091,34 +1091,34 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2023.11.28 00:49</t>
+          <t>2023.11.29 13:19</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2015.01</t>
+          <t>2040.87</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2023.11.28 05:04</t>
+          <t>2023.11.29 14:39</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2014.65</t>
+          <t>2038.11</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>1,08 USD</t>
+          <t>13,80 USD</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1133,34 +1133,34 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2023.11.28 00:49</t>
+          <t>2023.11.28 03:34</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2015.01</t>
+          <t>2017.19</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2023.11.28 05:04</t>
+          <t>2023.11.28 08:50</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2014.66</t>
+          <t>2012.56</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>1,05 USD</t>
+          <t>23,15 USD</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1175,34 +1175,34 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2023.11.27 10:01</t>
+          <t>2023.11.28 01:03</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2014.62</t>
+          <t>2017.23</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2023.11.27 14:43</t>
+          <t>2023.11.28 05:04</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2010.33</t>
+          <t>2014.6</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>25,74 USD</t>
+          <t>10,52 USD</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1217,27 +1217,27 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2023.11.27 09:11</t>
+          <t>2023.11.28 00:49</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2012.37</t>
+          <t>2015.01</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2023.11.27 14:42</t>
+          <t>2023.11.28 05:04</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2010.11</t>
+          <t>2014.65</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>11,30 USD</t>
+          <t>1,08 USD</t>
         </is>
       </c>
     </row>
@@ -1259,34 +1259,34 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2023.11.27 03:23</t>
+          <t>2023.11.28 00:49</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2008.45</t>
+          <t>2015.01</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2023.11.27 14:42</t>
+          <t>2023.11.28 05:04</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2010.18</t>
+          <t>2014.66</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>-5,19 USD</t>
+          <t>1,05 USD</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1301,34 +1301,34 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2023.11.27 04:45</t>
+          <t>2023.11.27 10:01</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2010.78</t>
+          <t>2014.62</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2023.11.27 14:42</t>
+          <t>2023.11.27 14:43</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2010.23</t>
+          <t>2010.33</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2,20 USD</t>
+          <t>25,74 USD</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1343,12 +1343,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2023.11.27 03:52</t>
+          <t>2023.11.27 09:11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2010.05</t>
+          <t>2012.37</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1358,19 +1358,19 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2009.98</t>
+          <t>2010.11</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0,28 USD</t>
+          <t>11,30 USD</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1385,34 +1385,34 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2023.11.27 02:28</t>
+          <t>2023.11.27 03:23</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2015.05</t>
+          <t>2008.45</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2023.11.27 03:21</t>
+          <t>2023.11.27 14:42</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2008.27</t>
+          <t>2010.18</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>40,68 USD</t>
+          <t>-5,19 USD</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1427,34 +1427,34 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2023.11.27 00:05</t>
+          <t>2023.11.27 04:45</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2000.91</t>
+          <t>2010.78</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2023.11.27 03:21</t>
+          <t>2023.11.27 14:42</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2008.35</t>
+          <t>2010.23</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>-22,32 USD</t>
+          <t>2,20 USD</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1469,34 +1469,34 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2023.11.27 02:11</t>
+          <t>2023.11.27 03:52</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2005.38</t>
+          <t>2010.05</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2023.11.27 03:21</t>
+          <t>2023.11.27 14:42</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2008.31</t>
+          <t>2009.98</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>-14,65 USD</t>
+          <t>0,28 USD</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1511,12 +1511,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2023.11.27 02:25</t>
+          <t>2023.11.27 02:28</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2009.56</t>
+          <t>2015.05</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1526,19 +1526,19 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2007.99</t>
+          <t>2008.27</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>7,85 USD</t>
+          <t>40,68 USD</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1548,39 +1548,39 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2023.11.24 17:01</t>
+          <t>2023.11.27 00:05</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1997.47</t>
+          <t>2000.91</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2023.11.24 17:27</t>
+          <t>2023.11.27 03:21</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1999.94</t>
+          <t>2008.35</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>12,35 USD</t>
+          <t>-22,32 USD</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1590,32 +1590,32 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2023.11.24 16:26</t>
+          <t>2023.11.27 02:11</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2000.19</t>
+          <t>2005.38</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2023.11.24 17:27</t>
+          <t>2023.11.27 03:21</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>1999.94</t>
+          <t>2008.31</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>-0,75 USD</t>
+          <t>-14,65 USD</t>
         </is>
       </c>
     </row>
@@ -1632,39 +1632,39 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2023.11.24 16:24</t>
+          <t>2023.11.27 02:25</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2000.68</t>
+          <t>2009.56</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2023.11.24 17:27</t>
+          <t>2023.11.27 03:21</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1999.94</t>
+          <t>2007.99</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>-3,70 USD</t>
+          <t>7,85 USD</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1679,27 +1679,27 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2023.11.24 16:31</t>
+          <t>2023.11.24 17:01</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1999.07</t>
+          <t>1997.47</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2023.11.24 17:26</t>
+          <t>2023.11.24 17:27</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>1999.95</t>
+          <t>1999.94</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>3,52 USD</t>
+          <t>12,35 USD</t>
         </is>
       </c>
     </row>
@@ -1716,39 +1716,39 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2023.11.24 16:10</t>
+          <t>2023.11.24 16:26</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2002.39</t>
+          <t>2000.19</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2023.11.24 16:22</t>
+          <t>2023.11.24 17:27</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2000.7</t>
+          <t>1999.94</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>5,07 USD</t>
+          <t>-0,75 USD</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1758,39 +1758,39 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2023.11.24 16:11</t>
+          <t>2023.11.24 16:24</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2002.32</t>
+          <t>2000.68</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2023.11.24 16:21</t>
+          <t>2023.11.24 17:27</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2000.96</t>
+          <t>1999.94</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>4,08 USD</t>
+          <t>-3,70 USD</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1805,34 +1805,34 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2023.11.24 08:35</t>
+          <t>2023.11.24 16:31</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1993.54</t>
+          <t>1999.07</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2023.11.24 11:20</t>
+          <t>2023.11.24 17:26</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>1995.9</t>
+          <t>1999.95</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>7,08 USD</t>
+          <t>3,52 USD</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1842,39 +1842,39 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2023.11.23 17:17</t>
+          <t>2023.11.24 16:10</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1990.53</t>
+          <t>2002.39</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2023.11.24 02:08</t>
+          <t>2023.11.24 16:22</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>1994.68</t>
+          <t>2000.7</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>20,75 USD</t>
+          <t>5,07 USD</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1884,32 +1884,32 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2023.11.23 13:25</t>
+          <t>2023.11.24 16:11</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1993.47</t>
+          <t>2002.32</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2023.11.24 02:08</t>
+          <t>2023.11.24 16:21</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1994.7</t>
+          <t>2000.96</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>6,15 USD</t>
+          <t>4,08 USD</t>
         </is>
       </c>
     </row>
@@ -1931,34 +1931,34 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2023.11.23 09:18</t>
+          <t>2023.11.24 08:35</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1995.83</t>
+          <t>1993.54</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2023.11.24 02:08</t>
+          <t>2023.11.24 11:20</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>1994.71</t>
+          <t>1995.9</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>-3,36 USD</t>
+          <t>7,08 USD</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1973,12 +1973,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2023.11.23 10:09</t>
+          <t>2023.11.23 17:17</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1994.2</t>
+          <t>1990.53</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1993,14 +1993,14 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>1,92 USD</t>
+          <t>20,75 USD</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2010,39 +2010,39 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2023.11.23 06:45</t>
+          <t>2023.11.23 13:25</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1995.43</t>
+          <t>1993.47</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2023.11.23 08:07</t>
+          <t>2023.11.24 02:08</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>1994.68</t>
+          <t>1994.7</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2,25 USD</t>
+          <t>6,15 USD</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2057,27 +2057,27 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2023.11.22 17:54</t>
+          <t>2023.11.23 09:18</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1990.96</t>
+          <t>1995.83</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2023.11.23 03:03</t>
+          <t>2023.11.24 02:08</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>1994.31</t>
+          <t>1994.71</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>16,75 USD</t>
+          <t>-3,36 USD</t>
         </is>
       </c>
     </row>
@@ -2099,34 +2099,34 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2023.11.22 16:46</t>
+          <t>2023.11.23 10:09</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1993.82</t>
+          <t>1994.2</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2023.11.23 03:03</t>
+          <t>2023.11.24 02:08</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>1994.31</t>
+          <t>1994.68</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>1,96 USD</t>
+          <t>1,92 USD</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2136,39 +2136,39 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2023.11.22 16:44</t>
+          <t>2023.11.23 06:45</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1995.42</t>
+          <t>1995.43</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2023.11.23 03:03</t>
+          <t>2023.11.23 08:07</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>1994.31</t>
+          <t>1994.68</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>-4,44 USD</t>
+          <t>2,25 USD</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2178,39 +2178,39 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2023.11.22 13:46</t>
+          <t>2023.11.22 17:54</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2003.05</t>
+          <t>1990.96</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2023.11.22 14:37</t>
+          <t>2023.11.23 03:03</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>1997.83</t>
+          <t>1994.31</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>20,88 USD</t>
+          <t>16,75 USD</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2220,39 +2220,39 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2023.11.22 12:33</t>
+          <t>2023.11.22 16:46</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2002.3</t>
+          <t>1993.82</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2023.11.22 14:37</t>
+          <t>2023.11.23 03:03</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>1997.79</t>
+          <t>1994.31</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>13,53 USD</t>
+          <t>1,96 USD</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2262,39 +2262,39 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2023.11.22 13:20</t>
+          <t>2023.11.22 16:44</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2001.71</t>
+          <t>1995.42</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2023.11.22 14:12</t>
+          <t>2023.11.23 03:03</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2001.16</t>
+          <t>1994.31</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>1,65 USD</t>
+          <t>-4,44 USD</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2309,34 +2309,34 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2023.11.21 14:29</t>
+          <t>2023.11.22 13:46</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1994.86</t>
+          <t>2003.05</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2023.11.21 14:42</t>
+          <t>2023.11.22 14:37</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>1994.23</t>
+          <t>1997.83</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>1,89 USD</t>
+          <t>20,88 USD</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2351,27 +2351,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2023.11.21 14:30</t>
+          <t>2023.11.22 12:33</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1998.23</t>
+          <t>2002.3</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2023.11.21 14:42</t>
+          <t>2023.11.22 14:37</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>1994.62</t>
+          <t>1997.79</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>14,44 USD</t>
+          <t>13,53 USD</t>
         </is>
       </c>
     </row>
@@ -2388,32 +2388,32 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2023.11.21 10:05</t>
+          <t>2023.11.22 13:20</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1987.24</t>
+          <t>2001.71</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2023.11.21 11:52</t>
+          <t>2023.11.22 14:12</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>1989</t>
+          <t>2001.16</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>5,28 USD</t>
+          <t>1,65 USD</t>
         </is>
       </c>
     </row>
@@ -2430,39 +2430,39 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2023.11.21 09:59</t>
+          <t>2023.11.21 14:29</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1987.9</t>
+          <t>1994.86</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2023.11.21 11:24</t>
+          <t>2023.11.21 14:42</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>1988.67</t>
+          <t>1994.23</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2,31 USD</t>
+          <t>1,89 USD</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2472,39 +2472,39 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2023.11.21 09:49</t>
+          <t>2023.11.21 14:30</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1988.49</t>
+          <t>1998.23</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2023.11.21 11:24</t>
+          <t>2023.11.21 14:42</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>1988.57</t>
+          <t>1994.62</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>0,24 USD</t>
+          <t>14,44 USD</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2514,32 +2514,32 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2023.11.21 04:52</t>
+          <t>2023.11.21 10:05</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1993.38</t>
+          <t>1987.24</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2023.11.21 09:46</t>
+          <t>2023.11.21 11:52</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>1989.3</t>
+          <t>1989</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>20,40 USD</t>
+          <t>5,28 USD</t>
         </is>
       </c>
     </row>
@@ -2556,32 +2556,32 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2023.11.21 03:08</t>
+          <t>2023.11.21 09:59</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1989.97</t>
+          <t>1987.9</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2023.11.21 09:46</t>
+          <t>2023.11.21 11:24</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>1989.57</t>
+          <t>1988.67</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>1,20 USD</t>
+          <t>2,31 USD</t>
         </is>
       </c>
     </row>
@@ -2598,39 +2598,39 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2023.11.21 02:24</t>
+          <t>2023.11.21 09:49</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1989.96</t>
+          <t>1988.49</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2023.11.21 09:46</t>
+          <t>2023.11.21 11:24</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>1989.72</t>
+          <t>1988.57</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>0,72 USD</t>
+          <t>0,24 USD</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2640,32 +2640,32 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2023.11.21 02:17</t>
+          <t>2023.11.21 04:52</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1988.15</t>
+          <t>1993.38</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2023.11.21 02:18</t>
+          <t>2023.11.21 09:46</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>1988.6</t>
+          <t>1989.3</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>1,35 USD</t>
+          <t>20,40 USD</t>
         </is>
       </c>
     </row>
@@ -2682,32 +2682,32 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2023.11.20 16:00</t>
+          <t>2023.11.21 03:08</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1969.83</t>
+          <t>1989.97</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2023.11.20 16:14</t>
+          <t>2023.11.21 09:46</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>1971.54</t>
+          <t>1989.57</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>5,13 USD</t>
+          <t>1,20 USD</t>
         </is>
       </c>
     </row>
@@ -2724,32 +2724,32 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2023.11.20 15:55</t>
+          <t>2023.11.21 02:24</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1970.88</t>
+          <t>1989.96</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2023.11.20 16:09</t>
+          <t>2023.11.21 09:46</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>1971.34</t>
+          <t>1989.72</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>1,38 USD</t>
+          <t>0,72 USD</t>
         </is>
       </c>
     </row>
@@ -2771,27 +2771,27 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2023.11.20 15:15</t>
+          <t>2023.11.21 02:17</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1967.01</t>
+          <t>1988.15</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2023.11.20 15:46</t>
+          <t>2023.11.21 02:18</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>1970.44</t>
+          <t>1988.6</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>10,29 USD</t>
+          <t>1,35 USD</t>
         </is>
       </c>
     </row>
@@ -2813,27 +2813,27 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2023.11.20 14:36</t>
+          <t>2023.11.20 16:00</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1967.02</t>
+          <t>1969.83</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2023.11.20 15:45</t>
+          <t>2023.11.20 16:14</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>1970.42</t>
+          <t>1971.54</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>10,20 USD</t>
+          <t>5,13 USD</t>
         </is>
       </c>
     </row>
@@ -2855,27 +2855,27 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2023.11.20 15:35</t>
+          <t>2023.11.20 15:55</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1967.4</t>
+          <t>1970.88</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2023.11.20 15:42</t>
+          <t>2023.11.20 16:09</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>1969</t>
+          <t>1971.34</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>4,80 USD</t>
+          <t>1,38 USD</t>
         </is>
       </c>
     </row>
@@ -2897,27 +2897,27 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2023.11.20 15:14</t>
+          <t>2023.11.20 15:15</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1967.84</t>
+          <t>1967.01</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2023.11.20 15:40</t>
+          <t>2023.11.20 15:46</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>1968.26</t>
+          <t>1970.44</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>1,26 USD</t>
+          <t>10,29 USD</t>
         </is>
       </c>
     </row>
@@ -2934,39 +2934,39 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2023.11.20 04:18</t>
+          <t>2023.11.20 14:36</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1981.37</t>
+          <t>1967.02</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2023.11.20 09:21</t>
+          <t>2023.11.20 15:45</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>1977.65</t>
+          <t>1970.42</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>11,16 USD</t>
+          <t>10,20 USD</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2976,32 +2976,32 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2023.11.20 03:34</t>
+          <t>2023.11.20 15:35</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>1984.71</t>
+          <t>1967.4</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2023.11.20 04:14</t>
+          <t>2023.11.20 15:42</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>1980.39</t>
+          <t>1969</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>17,28 USD</t>
+          <t>4,80 USD</t>
         </is>
       </c>
     </row>
@@ -3018,39 +3018,39 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2023.11.20 02:11</t>
+          <t>2023.11.20 15:14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1980.66</t>
+          <t>1967.84</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2023.11.20 04:14</t>
+          <t>2023.11.20 15:40</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>1980.42</t>
+          <t>1968.26</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>0,72 USD</t>
+          <t>1,26 USD</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -3065,34 +3065,34 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2023.11.20 02:10</t>
+          <t>2023.11.20 04:18</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1980.57</t>
+          <t>1981.37</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2023.11.20 02:12</t>
+          <t>2023.11.20 09:21</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>1980.29</t>
+          <t>1977.65</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>1,40 USD</t>
+          <t>11,16 USD</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3107,34 +3107,34 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2023.11.17 13:33</t>
+          <t>2023.11.20 03:34</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1990.09</t>
+          <t>1984.71</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2023.11.17 14:49</t>
+          <t>2023.11.20 04:14</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>1984.86</t>
+          <t>1980.39</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>31,38 USD</t>
+          <t>17,28 USD</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3149,34 +3149,34 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2023.11.17 10:07</t>
+          <t>2023.11.20 02:11</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1989.92</t>
+          <t>1980.66</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2023.11.17 14:49</t>
+          <t>2023.11.20 04:14</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>1984.87</t>
+          <t>1980.42</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>30,30 USD</t>
+          <t>0,72 USD</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3191,34 +3191,34 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2023.11.16 15:56</t>
+          <t>2023.11.20 02:10</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1979.9</t>
+          <t>1980.57</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2023.11.17 14:49</t>
+          <t>2023.11.20 02:12</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>1984.9</t>
+          <t>1980.29</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>-15,00 USD</t>
+          <t>1,40 USD</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3233,12 +3233,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2023.11.16 17:06</t>
+          <t>2023.11.17 13:33</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1986.43</t>
+          <t>1990.09</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3248,19 +3248,19 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>1984.83</t>
+          <t>1984.86</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>8,00 USD</t>
+          <t>31,38 USD</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3275,12 +3275,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2023.11.17 08:32</t>
+          <t>2023.11.17 10:07</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1984.96</t>
+          <t>1989.92</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3290,19 +3290,19 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>1984.77</t>
+          <t>1984.87</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>0,95 USD</t>
+          <t>30,30 USD</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3317,12 +3317,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2023.11.17 03:09</t>
+          <t>2023.11.16 15:56</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1984.8</t>
+          <t>1979.9</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3332,19 +3332,19 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>1984.61</t>
+          <t>1984.9</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>1,14 USD</t>
+          <t>-15,00 USD</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3359,27 +3359,27 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2023.11.16 16:20</t>
+          <t>2023.11.16 17:06</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1984.67</t>
+          <t>1986.43</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2023.11.17 07:33</t>
+          <t>2023.11.17 14:49</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>1983.99</t>
+          <t>1984.83</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>2,72 USD</t>
+          <t>8,00 USD</t>
         </is>
       </c>
     </row>
@@ -3401,34 +3401,34 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2023.11.16 19:10</t>
+          <t>2023.11.17 08:32</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1984.27</t>
+          <t>1984.96</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2023.11.17 07:33</t>
+          <t>2023.11.17 14:49</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>1984.04</t>
+          <t>1984.77</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>1,15 USD</t>
+          <t>0,95 USD</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3438,39 +3438,39 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2023.11.16 11:36</t>
+          <t>2023.11.17 03:09</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1965.57</t>
+          <t>1984.8</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2023.11.16 14:30</t>
+          <t>2023.11.17 14:49</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>1969.68</t>
+          <t>1984.61</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>12,33 USD</t>
+          <t>1,14 USD</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3480,39 +3480,39 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2023.11.16 07:51</t>
+          <t>2023.11.16 16:20</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1966.42</t>
+          <t>1984.67</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2023.11.16 14:30</t>
+          <t>2023.11.17 07:33</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>1969.68</t>
+          <t>1983.99</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>9,78 USD</t>
+          <t>2,72 USD</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3522,32 +3522,32 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2023.11.16 05:04</t>
+          <t>2023.11.16 19:10</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1961.26</t>
+          <t>1984.27</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2023.11.16 06:12</t>
+          <t>2023.11.17 07:33</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>1963.33</t>
+          <t>1984.04</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>6,21 USD</t>
+          <t>1,15 USD</t>
         </is>
       </c>
     </row>
@@ -3564,32 +3564,32 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2023.11.15 14:49</t>
+          <t>2023.11.16 11:36</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1965.77</t>
+          <t>1965.57</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2023.11.15 15:10</t>
+          <t>2023.11.16 14:30</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>1964.25</t>
+          <t>1969.68</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>4,56 USD</t>
+          <t>12,33 USD</t>
         </is>
       </c>
     </row>
@@ -3606,39 +3606,39 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2023.11.15 14:52</t>
+          <t>2023.11.16 07:51</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1966.08</t>
+          <t>1966.42</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2023.11.15 15:10</t>
+          <t>2023.11.16 14:30</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>1964.23</t>
+          <t>1969.68</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>5,55 USD</t>
+          <t>9,78 USD</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3648,32 +3648,32 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2023.11.15 09:53</t>
+          <t>2023.11.16 05:04</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1971.11</t>
+          <t>1961.26</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2023.11.15 14:37</t>
+          <t>2023.11.16 06:12</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>1966.74</t>
+          <t>1963.33</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>17,48 USD</t>
+          <t>6,21 USD</t>
         </is>
       </c>
     </row>
@@ -3695,27 +3695,27 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2023.11.15 07:22</t>
+          <t>2023.11.15 14:49</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1968.12</t>
+          <t>1965.77</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2023.11.15 14:36</t>
+          <t>2023.11.15 15:10</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>1967.3</t>
+          <t>1964.25</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>2,46 USD</t>
+          <t>4,56 USD</t>
         </is>
       </c>
     </row>
@@ -3732,39 +3732,39 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2023.11.15 01:18</t>
+          <t>2023.11.15 14:52</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1962.04</t>
+          <t>1966.08</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2023.11.15 04:46</t>
+          <t>2023.11.15 15:10</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>1966.58</t>
+          <t>1964.23</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>13,62 USD</t>
+          <t>5,55 USD</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3774,32 +3774,32 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2023.11.14 14:50</t>
+          <t>2023.11.15 09:53</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1953.74</t>
+          <t>1971.11</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2023.11.14 14:54</t>
+          <t>2023.11.15 14:37</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>1956.11</t>
+          <t>1966.74</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>7,11 USD</t>
+          <t>17,48 USD</t>
         </is>
       </c>
     </row>
@@ -3816,32 +3816,32 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2023.11.14 14:37</t>
+          <t>2023.11.15 07:22</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1954.07</t>
+          <t>1968.12</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2023.11.14 14:41</t>
+          <t>2023.11.15 14:36</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>1957.38</t>
+          <t>1967.3</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>9,93 USD</t>
+          <t>2,46 USD</t>
         </is>
       </c>
     </row>
@@ -3863,27 +3863,27 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2023.11.14 14:36</t>
+          <t>2023.11.15 01:18</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1955.58</t>
+          <t>1962.04</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2023.11.14 14:41</t>
+          <t>2023.11.15 04:46</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>1956.9</t>
+          <t>1966.58</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>3,96 USD</t>
+          <t>13,62 USD</t>
         </is>
       </c>
     </row>
@@ -3905,34 +3905,34 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2023.11.14 03:04</t>
+          <t>2023.11.14 14:50</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1945.46</t>
+          <t>1953.74</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2023.11.14 14:30</t>
+          <t>2023.11.14 14:54</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>1952</t>
+          <t>1956.11</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>19,62 USD</t>
+          <t>7,11 USD</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3947,34 +3947,34 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2023.11.10 08:22</t>
+          <t>2023.11.14 14:37</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1955.12</t>
+          <t>1954.07</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2023.11.13 17:36</t>
+          <t>2023.11.14 14:41</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>1945.52</t>
+          <t>1957.38</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>-38,40 USD</t>
+          <t>9,93 USD</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0,07</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3989,34 +3989,34 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2023.11.13 15:04</t>
+          <t>2023.11.14 14:36</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1934.95</t>
+          <t>1955.58</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2023.11.13 17:36</t>
+          <t>2023.11.14 14:41</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>1945.66</t>
+          <t>1956.9</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>74,97 USD</t>
+          <t>3,96 USD</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>0,07</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4031,34 +4031,34 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2023.11.13 15:49</t>
+          <t>2023.11.14 03:04</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1933.79</t>
+          <t>1945.46</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2023.11.13 17:36</t>
+          <t>2023.11.14 14:30</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>1945.65</t>
+          <t>1952</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>83,02 USD</t>
+          <t>19,62 USD</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4073,12 +4073,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2023.11.10 12:29</t>
+          <t>2023.11.10 08:22</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1948.74</t>
+          <t>1955.12</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -4088,19 +4088,19 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>1945.76</t>
+          <t>1945.52</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>-17,88 USD</t>
+          <t>-38,40 USD</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,07</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -4115,12 +4115,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2023.11.10 05:36</t>
+          <t>2023.11.13 15:04</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1957.84</t>
+          <t>1934.95</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -4130,12 +4130,12 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>1945.76</t>
+          <t>1945.66</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>-36,24 USD</t>
+          <t>74,97 USD</t>
         </is>
       </c>
     </row>
@@ -4157,12 +4157,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2023.11.13 04:25</t>
+          <t>2023.11.13 15:49</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1935.24</t>
+          <t>1933.79</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -4172,12 +4172,12 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>1945.76</t>
+          <t>1945.65</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>73,64 USD</t>
+          <t>83,02 USD</t>
         </is>
       </c>
     </row>
@@ -4199,12 +4199,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2023.11.10 15:57</t>
+          <t>2023.11.10 12:29</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1942.48</t>
+          <t>1948.74</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -4214,12 +4214,12 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>1945.77</t>
+          <t>1945.76</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>19,74 USD</t>
+          <t>-17,88 USD</t>
         </is>
       </c>
     </row>
@@ -4241,12 +4241,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2023.11.10 05:37</t>
+          <t>2023.11.10 05:36</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1957.76</t>
+          <t>1957.84</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4256,12 +4256,12 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>1945.77</t>
+          <t>1945.76</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>-35,97 USD</t>
+          <t>-36,24 USD</t>
         </is>
       </c>
     </row>
@@ -4283,12 +4283,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2023.11.13 16:35</t>
+          <t>2023.11.13 04:25</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1935.1</t>
+          <t>1935.24</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4298,12 +4298,12 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>1945.86</t>
+          <t>1945.76</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>75,32 USD</t>
+          <t>73,64 USD</t>
         </is>
       </c>
     </row>
@@ -4325,34 +4325,34 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2023.11.10 13:44</t>
+          <t>2023.11.10 15:57</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1945.05</t>
+          <t>1942.48</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2023.11.13 17:34</t>
+          <t>2023.11.13 17:36</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>1945.27</t>
+          <t>1945.77</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>1,32 USD</t>
+          <t>19,74 USD</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>0,07</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -4367,34 +4367,34 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2023.11.13 04:25</t>
+          <t>2023.11.10 05:37</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1935.43</t>
+          <t>1957.76</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2023.11.13 16:47</t>
+          <t>2023.11.13 17:36</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>1937.01</t>
+          <t>1945.77</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>11,06 USD</t>
+          <t>-35,97 USD</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,07</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -4409,34 +4409,34 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2023.11.13 13:56</t>
+          <t>2023.11.13 16:35</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1936.01</t>
+          <t>1935.1</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2023.11.13 16:18</t>
+          <t>2023.11.13 17:36</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>1936.28</t>
+          <t>1945.86</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>1,62 USD</t>
+          <t>75,32 USD</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -4446,39 +4446,39 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2023.11.13 03:16</t>
+          <t>2023.11.10 13:44</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1940.12</t>
+          <t>1945.05</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2023.11.13 04:19</t>
+          <t>2023.11.13 17:34</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>1934.86</t>
+          <t>1945.27</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>21,04 USD</t>
+          <t>1,32 USD</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,07</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -4488,39 +4488,39 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2023.11.13 03:23</t>
+          <t>2023.11.13 04:25</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1940.64</t>
+          <t>1935.43</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2023.11.13 04:19</t>
+          <t>2023.11.13 16:47</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>1934.86</t>
+          <t>1937.01</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>23,12 USD</t>
+          <t>11,06 USD</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -4530,39 +4530,39 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2023.11.13 03:16</t>
+          <t>2023.11.13 13:56</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>1940.12</t>
+          <t>1936.01</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2023.11.13 04:19</t>
+          <t>2023.11.13 16:18</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>1934.86</t>
+          <t>1936.28</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>21,04 USD</t>
+          <t>1,62 USD</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>0,07</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -4572,39 +4572,39 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2023.11.10 17:36</t>
+          <t>2023.11.13 03:16</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>1937.69</t>
+          <t>1940.12</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2023.11.13 03:22</t>
+          <t>2023.11.13 04:19</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>1940.67</t>
+          <t>1934.86</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>20,86 USD</t>
+          <t>21,04 USD</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -4614,39 +4614,39 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2023.11.09 09:27</t>
+          <t>2023.11.13 03:23</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1946.61</t>
+          <t>1940.64</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2023.11.09 16:39</t>
+          <t>2023.11.13 04:19</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>1961.8</t>
+          <t>1934.86</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>91,14 USD</t>
+          <t>23,12 USD</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -4656,32 +4656,32 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2023.11.08 18:38</t>
+          <t>2023.11.13 03:16</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1953.09</t>
+          <t>1940.12</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2023.11.09 16:39</t>
+          <t>2023.11.13 04:19</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>1961.8</t>
+          <t>1934.86</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>52,26 USD</t>
+          <t>21,04 USD</t>
         </is>
       </c>
     </row>
@@ -4703,34 +4703,34 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2023.11.09 05:29</t>
+          <t>2023.11.10 17:36</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1949.13</t>
+          <t>1937.69</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2023.11.09 16:39</t>
+          <t>2023.11.13 03:22</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>1961.89</t>
+          <t>1940.67</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>89,32 USD</t>
+          <t>20,86 USD</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>0,05</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -4745,12 +4745,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2023.11.08 11:32</t>
+          <t>2023.11.09 09:27</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>1960.93</t>
+          <t>1946.61</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -4760,12 +4760,12 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>1961.81</t>
+          <t>1961.8</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>4,40 USD</t>
+          <t>91,14 USD</t>
         </is>
       </c>
     </row>
@@ -4787,12 +4787,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2023.11.08 17:37</t>
+          <t>2023.11.08 18:38</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>1957.46</t>
+          <t>1953.09</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4802,19 +4802,19 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>1962.01</t>
+          <t>1961.8</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>27,30 USD</t>
+          <t>52,26 USD</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,07</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -4829,12 +4829,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2023.11.08 10:36</t>
+          <t>2023.11.09 05:29</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>1966.69</t>
+          <t>1949.13</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4844,19 +4844,19 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>1962.12</t>
+          <t>1961.89</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>-18,28 USD</t>
+          <t>89,32 USD</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>0,06</t>
+          <t>0,05</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -4871,12 +4871,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2023.11.08 16:53</t>
+          <t>2023.11.08 11:32</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>1955.95</t>
+          <t>1960.93</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4886,19 +4886,19 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>1961.87</t>
+          <t>1961.81</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>35,52 USD</t>
+          <t>4,40 USD</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -4913,12 +4913,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2023.11.08 02:17</t>
+          <t>2023.11.08 17:37</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1969.54</t>
+          <t>1957.46</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4928,19 +4928,19 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>1961.87</t>
+          <t>1962.01</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>-23,01 USD</t>
+          <t>27,30 USD</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -4955,12 +4955,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2023.11.08 07:06</t>
+          <t>2023.11.08 10:36</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1965.88</t>
+          <t>1966.69</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4970,19 +4970,19 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>1961.88</t>
+          <t>1962.12</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>-12,00 USD</t>
+          <t>-18,28 USD</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,06</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -4992,32 +4992,32 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2023.11.08 18:11</t>
+          <t>2023.11.08 16:53</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>1955.93</t>
+          <t>1955.95</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2023.11.08 18:37</t>
+          <t>2023.11.09 16:39</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>1952.68</t>
+          <t>1961.87</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>9,75 USD</t>
+          <t>35,52 USD</t>
         </is>
       </c>
     </row>
@@ -5034,39 +5034,39 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>sell</t>
+          <t>buy</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2023.11.08 17:59</t>
+          <t>2023.11.08 02:17</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>1954.52</t>
+          <t>1969.54</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2023.11.08 18:24</t>
+          <t>2023.11.09 16:39</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>1953.3</t>
+          <t>1961.87</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>3,66 USD</t>
+          <t>-23,01 USD</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>0,04</t>
+          <t>0,03</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -5081,27 +5081,27 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2023.11.07 13:34</t>
+          <t>2023.11.08 07:06</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>1961.66</t>
+          <t>1965.88</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2023.11.07 19:22</t>
+          <t>2023.11.09 16:39</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>1966.41</t>
+          <t>1961.88</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>19,00 USD</t>
+          <t>-12,00 USD</t>
         </is>
       </c>
     </row>
@@ -5118,32 +5118,32 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2023.11.07 10:03</t>
+          <t>2023.11.08 18:11</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1965.38</t>
+          <t>1955.93</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2023.11.07 19:22</t>
+          <t>2023.11.08 18:37</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>1966.41</t>
+          <t>1952.68</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>3,09 USD</t>
+          <t>9,75 USD</t>
         </is>
       </c>
     </row>
@@ -5160,39 +5160,39 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>buy</t>
+          <t>sell</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2023.11.07 08:53</t>
+          <t>2023.11.08 17:59</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1969.74</t>
+          <t>1954.52</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2023.11.07 19:22</t>
+          <t>2023.11.08 18:24</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>1966.41</t>
+          <t>1953.3</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>-9,99 USD</t>
+          <t>3,66 USD</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>0,03</t>
+          <t>0,04</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -5207,27 +5207,27 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2023.11.06 17:01</t>
+          <t>2023.11.07 13:34</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>1980.68</t>
+          <t>1961.66</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>2023.11.06 18:07</t>
+          <t>2023.11.07 19:22</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>1984.25</t>
+          <t>1966.41</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>10,71 USD</t>
+          <t>19,00 USD</t>
         </is>
       </c>
     </row>
@@ -5249,27 +5249,27 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2023.11.06 16:57</t>
+          <t>2023.11.07 10:03</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>1982.25</t>
+          <t>1965.38</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2023.11.06 17:57</t>
+          <t>2023.11.07 19:22</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>1966.41</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>5,25 USD</t>
+          <t>3,09 USD</t>
         </is>
       </c>
     </row>
@@ -5291,27 +5291,27 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2023.11.06 16:45</t>
+          <t>2023.11.07 08:53</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>1983.89</t>
+          <t>1969.74</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2023.11.06 17:57</t>
+          <t>2023.11.07 19:22</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>1966.41</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>0,33 USD</t>
+          <t>-9,99 USD</t>
         </is>
       </c>
     </row>
@@ -5328,30 +5328,156 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2023.11.06 17:01</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>1980.68</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>2023.11.06 18:07</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>1984.25</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>10,71 USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>0,03</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2023.11.06 16:57</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>1982.25</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>2023.11.06 17:57</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>1984</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>5,25 USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>0,03</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2023.11.06 16:45</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>1983.89</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>2023.11.06 17:57</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>1984</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>0,33 USD</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>0,03</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>GOLD</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
           <t>sell</t>
         </is>
       </c>
-      <c r="D117" t="inlineStr">
+      <c r="D120" t="inlineStr">
         <is>
           <t>2023.11.06 14:24</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
+      <c r="E120" t="inlineStr">
         <is>
           <t>1986.77</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr">
+      <c r="F120" t="inlineStr">
         <is>
           <t>2023.11.06 16:34</t>
         </is>
       </c>
-      <c r="G117" t="inlineStr">
+      <c r="G120" t="inlineStr">
         <is>
           <t>1984.26</t>
         </is>
       </c>
-      <c r="H117" t="inlineStr">
+      <c r="H120" t="inlineStr">
         <is>
           <t>7,53 USD</t>
         </is>

</xml_diff>